<commit_message>
Major bugfix. Now working fine
</commit_message>
<xml_diff>
--- a/ML_Offline3/ALS/Results_1305003.xlsx
+++ b/ML_Offline3/ALS/Results_1305003.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Google Drive\Course BUET\CSE471_Jan'18\CSE_472_Assignment_3_Recommender_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="10_ncr:8100000_{FFBBA718-B29C-4D6D-B86D-AE079B601B13}" xr6:coauthVersionLast="35" xr6:coauthVersionMax="35" xr10:uidLastSave="{47DC3616-6FE8-4D38-9011-FD91DA29BA42}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="10_ncr:8100000_{FFBBA718-B29C-4D6D-B86D-AE079B601B13}" xr6:coauthVersionLast="35" xr6:coauthVersionMax="35" xr10:uidLastSave="{F30FF275-53E6-4126-9B8F-757D4DD57F9C}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{2B0C9EB4-8911-4EF6-82FF-D91E08F8A887}"/>
   </bookViews>
@@ -110,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -119,6 +119,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="সাধারণ" xfId="0" builtinId="0"/>
@@ -435,8 +436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A0B9AC5-2F9A-408B-B177-39C14F460105}">
   <dimension ref="B3:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{DBC058CB-A56B-54E3-8BC7-4C948B65D9A9}">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0" xr3:uid="{DBC058CB-A56B-54E3-8BC7-4C948B65D9A9}">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -479,16 +480,16 @@
         <v>10</v>
       </c>
       <c r="C5" s="4">
-        <v>3.0344000000000002</v>
+        <v>3.7362000000000002</v>
       </c>
       <c r="D5" s="4">
-        <v>3.0344000000000002</v>
+        <v>3.9727000000000001</v>
       </c>
       <c r="E5" s="4">
-        <v>3.0344000000000002</v>
+        <v>3.6125882765697899</v>
       </c>
       <c r="F5" s="4">
-        <v>3.0343</v>
+        <v>2.8656999999999999</v>
       </c>
     </row>
     <row r="6" spans="2:6">
@@ -496,16 +497,16 @@
         <v>20</v>
       </c>
       <c r="C6" s="4">
-        <v>3.0348999999999999</v>
+        <v>9.7098999999999993</v>
       </c>
       <c r="D6" s="4">
-        <v>3.0348999999999999</v>
+        <v>8.7521000000000004</v>
       </c>
       <c r="E6" s="4">
-        <v>3.0345</v>
+        <v>5.7435999999999998</v>
       </c>
       <c r="F6" s="4">
-        <v>3.0343</v>
+        <v>2.669</v>
       </c>
     </row>
     <row r="7" spans="2:6">
@@ -513,16 +514,16 @@
         <v>40</v>
       </c>
       <c r="C7" s="4">
-        <v>3.0394999999999999</v>
+        <v>27.6129</v>
       </c>
       <c r="D7" s="4">
-        <v>3.0381999999999998</v>
+        <v>23.088999999999999</v>
       </c>
       <c r="E7" s="4">
-        <v>3.0348000000000002</v>
+        <v>8.0867000000000004</v>
       </c>
       <c r="F7" s="4">
-        <v>3.0343</v>
+        <v>2.5977999999999999</v>
       </c>
     </row>
     <row r="10" spans="2:6">
@@ -558,16 +559,16 @@
         <v>10</v>
       </c>
       <c r="C12" s="4">
-        <v>2.9601000000000002</v>
+        <v>2.7580867267323499</v>
       </c>
       <c r="D12" s="4">
-        <v>2.9601000000000002</v>
+        <v>2.7245297198935998</v>
       </c>
       <c r="E12" s="4">
-        <v>2.9601000000000002</v>
+        <v>2.8170806007557299</v>
       </c>
       <c r="F12" s="4">
-        <v>2.9601000000000002</v>
+        <v>2.7148187709613101</v>
       </c>
     </row>
     <row r="13" spans="2:6">
@@ -575,16 +576,16 @@
         <v>20</v>
       </c>
       <c r="C13" s="4">
-        <v>2.96</v>
+        <v>2.55016</v>
       </c>
       <c r="D13" s="4">
-        <v>2.9601000000000002</v>
+        <v>2.6207207634949401</v>
       </c>
       <c r="E13" s="4">
-        <v>2.96</v>
+        <v>2.4481518697826301</v>
       </c>
       <c r="F13" s="4">
-        <v>2.96</v>
+        <v>2.4806417943242001</v>
       </c>
     </row>
     <row r="14" spans="2:6">
@@ -592,16 +593,16 @@
         <v>40</v>
       </c>
       <c r="C14" s="4">
-        <v>2.9599000000000002</v>
+        <v>2.1398590372275899</v>
       </c>
       <c r="D14" s="4">
-        <v>2.9599000000000002</v>
-      </c>
-      <c r="E14" s="4">
-        <v>2.9599000000000002</v>
+        <v>1.98245689810242</v>
+      </c>
+      <c r="E14" s="6">
+        <v>1.9585765614249799</v>
       </c>
       <c r="F14" s="4">
-        <v>2.9599000000000002</v>
+        <v>2.2333437272225001</v>
       </c>
     </row>
     <row r="17" spans="2:6">

</xml_diff>